<commit_message>
got rid of a circular reference in 2011 Jan Data
</commit_message>
<xml_diff>
--- a/Kevin/Analysis.xlsx
+++ b/Kevin/Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="2011 Analysis" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2577" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="1004">
   <si>
     <t>Months:</t>
   </si>
@@ -3036,6 +3036,9 @@
   </si>
   <si>
     <t># of Major Contributors</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -3315,7 +3318,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>49.646959715186867</c:v>
+                  <c:v>49.585161390707462</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70.445705838563896</c:v>
@@ -3492,8 +3495,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="658832168"/>
-        <c:axId val="658832560"/>
+        <c:axId val="303834640"/>
+        <c:axId val="303831112"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3604,7 +3607,7 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="12"/>
                       <c:pt idx="0">
-                        <c:v>49.646959715186867</c:v>
+                        <c:v>49.585161390707462</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>70.445705838563896</c:v>
@@ -3651,7 +3654,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2011 Analysis'!$A$4</c15:sqref>
@@ -3692,7 +3695,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2011 Analysis'!$B$2:$M$2</c15:sqref>
@@ -3742,7 +3745,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2011 Analysis'!$B$4:$M$4</c15:sqref>
@@ -3798,7 +3801,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="658832168"/>
+        <c:axId val="303834640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3854,12 +3857,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="658832560"/>
+        <c:crossAx val="303831112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="658832560"/>
+        <c:axId val="303831112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3916,7 +3919,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="658832168"/>
+        <c:crossAx val="303834640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4223,11 +4226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593219208"/>
-        <c:axId val="593217640"/>
+        <c:axId val="362708152"/>
+        <c:axId val="362708936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593219208"/>
+        <c:axId val="362708152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4340,12 +4343,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593217640"/>
+        <c:crossAx val="362708936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593217640"/>
+        <c:axId val="362708936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4458,7 +4461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593219208"/>
+        <c:crossAx val="362708152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4645,7 +4648,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>49.646959715186867</c:v>
+                  <c:v>49.585161390707462</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70.445705838563896</c:v>
@@ -4738,11 +4741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="478896904"/>
-        <c:axId val="478904352"/>
+        <c:axId val="362712464"/>
+        <c:axId val="362713248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="478896904"/>
+        <c:axId val="362712464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4860,12 +4863,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478904352"/>
+        <c:crossAx val="362713248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="478904352"/>
+        <c:axId val="362713248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4978,7 +4981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478896904"/>
+        <c:crossAx val="362712464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5171,11 +5174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593252528"/>
-        <c:axId val="593242728"/>
+        <c:axId val="303836992"/>
+        <c:axId val="303837384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593252528"/>
+        <c:axId val="303836992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,12 +5290,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593242728"/>
+        <c:crossAx val="303837384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593242728"/>
+        <c:axId val="303837384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5405,7 +5408,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593252528"/>
+        <c:crossAx val="303836992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5642,11 +5645,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593241552"/>
-        <c:axId val="593245080"/>
+        <c:axId val="363184192"/>
+        <c:axId val="363189680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593241552"/>
+        <c:axId val="363184192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5702,12 +5705,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593245080"/>
+        <c:crossAx val="363189680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593245080"/>
+        <c:axId val="363189680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5764,7 +5767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593241552"/>
+        <c:crossAx val="363184192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6160,11 +6163,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593241160"/>
-        <c:axId val="593243512"/>
+        <c:axId val="363188504"/>
+        <c:axId val="363186544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593241160"/>
+        <c:axId val="363188504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6220,12 +6223,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593243512"/>
+        <c:crossAx val="363186544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593243512"/>
+        <c:axId val="363186544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6282,7 +6285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593241160"/>
+        <c:crossAx val="363188504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6408,7 +6411,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6622,11 +6624,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593244688"/>
-        <c:axId val="593243120"/>
+        <c:axId val="363187328"/>
+        <c:axId val="363182624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593244688"/>
+        <c:axId val="363187328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6682,12 +6684,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593243120"/>
+        <c:crossAx val="363182624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593243120"/>
+        <c:axId val="363182624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6744,7 +6746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593244688"/>
+        <c:crossAx val="363187328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6758,7 +6760,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6871,7 +6872,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7302,11 +7302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593249000"/>
-        <c:axId val="593244296"/>
+        <c:axId val="363188112"/>
+        <c:axId val="363190072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593249000"/>
+        <c:axId val="363188112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7362,12 +7362,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593244296"/>
+        <c:crossAx val="363190072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593244296"/>
+        <c:axId val="363190072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7424,7 +7424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593249000"/>
+        <c:crossAx val="363188112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7438,7 +7438,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7764,11 +7763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593249784"/>
-        <c:axId val="593250176"/>
+        <c:axId val="363183408"/>
+        <c:axId val="363183800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593249784"/>
+        <c:axId val="363183408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7810,12 +7809,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593250176"/>
+        <c:crossAx val="363183800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593250176"/>
+        <c:axId val="363183800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7866,7 +7865,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593249784"/>
+        <c:crossAx val="363183408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7994,7 +7993,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8381,11 +8379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593246256"/>
-        <c:axId val="593247040"/>
+        <c:axId val="363188896"/>
+        <c:axId val="363185368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593246256"/>
+        <c:axId val="363188896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8441,12 +8439,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593247040"/>
+        <c:crossAx val="363185368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593247040"/>
+        <c:axId val="363185368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8503,7 +8501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593246256"/>
+        <c:crossAx val="363188896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8517,7 +8515,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8629,7 +8626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8843,11 +8839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593251352"/>
-        <c:axId val="593253704"/>
+        <c:axId val="363185760"/>
+        <c:axId val="363394168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593251352"/>
+        <c:axId val="363185760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8889,12 +8885,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593253704"/>
+        <c:crossAx val="363394168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593253704"/>
+        <c:axId val="363394168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8945,7 +8941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593251352"/>
+        <c:crossAx val="363185760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8959,7 +8955,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9195,11 +9190,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276833016"/>
-        <c:axId val="276834192"/>
+        <c:axId val="303831896"/>
+        <c:axId val="303835424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276833016"/>
+        <c:axId val="303831896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9311,12 +9306,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276834192"/>
+        <c:crossAx val="303835424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276834192"/>
+        <c:axId val="303835424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9434,7 +9429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276833016"/>
+        <c:crossAx val="303831896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9723,11 +9718,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="646955872"/>
-        <c:axId val="646957440"/>
+        <c:axId val="363401616"/>
+        <c:axId val="363399656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="646955872"/>
+        <c:axId val="363401616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9845,12 +9840,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646957440"/>
+        <c:crossAx val="363399656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="646957440"/>
+        <c:axId val="363399656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9963,7 +9958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646955872"/>
+        <c:crossAx val="363401616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10060,7 +10055,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10246,11 +10240,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="646914304"/>
-        <c:axId val="646908424"/>
+        <c:axId val="363395736"/>
+        <c:axId val="363396520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="646914304"/>
+        <c:axId val="363395736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10301,7 +10295,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10368,12 +10361,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646908424"/>
+        <c:crossAx val="363396520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="646908424"/>
+        <c:axId val="363396520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10419,7 +10412,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10486,7 +10478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646914304"/>
+        <c:crossAx val="363395736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10583,7 +10575,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10769,11 +10760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="686131944"/>
-        <c:axId val="686131160"/>
+        <c:axId val="363398088"/>
+        <c:axId val="363396128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="686131944"/>
+        <c:axId val="363398088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10824,7 +10815,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10891,12 +10881,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686131160"/>
+        <c:crossAx val="363396128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="686131160"/>
+        <c:axId val="363396128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10942,7 +10932,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11009,7 +10998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686131944"/>
+        <c:crossAx val="363398088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11223,7 +11212,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>49.646959715186867</c:v>
+                  <c:v>49.585161390707462</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70.445705838563896</c:v>
@@ -11271,11 +11260,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276834584"/>
-        <c:axId val="276834976"/>
+        <c:axId val="303836208"/>
+        <c:axId val="303838168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276834584"/>
+        <c:axId val="303836208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11387,12 +11376,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276834976"/>
+        <c:crossAx val="303838168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276834976"/>
+        <c:axId val="303838168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11505,7 +11494,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276834584"/>
+        <c:crossAx val="303836208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11813,11 +11802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="646911560"/>
-        <c:axId val="646910776"/>
+        <c:axId val="303833072"/>
+        <c:axId val="303832288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="646911560"/>
+        <c:axId val="303833072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11873,12 +11862,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646910776"/>
+        <c:crossAx val="303832288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="646910776"/>
+        <c:axId val="303832288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11935,7 +11924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646911560"/>
+        <c:crossAx val="303833072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12275,11 +12264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="593226656"/>
-        <c:axId val="593227440"/>
+        <c:axId val="303836600"/>
+        <c:axId val="362715208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="593226656"/>
+        <c:axId val="303836600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12336,12 +12325,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593227440"/>
+        <c:crossAx val="362715208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="593227440"/>
+        <c:axId val="362715208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12398,7 +12387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593226656"/>
+        <c:crossAx val="303836600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12688,7 +12677,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>49.646959715186867</c:v>
+                  <c:v>49.585161390707462</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70.445705838563896</c:v>
@@ -12821,11 +12810,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="628429872"/>
-        <c:axId val="628428304"/>
+        <c:axId val="362707760"/>
+        <c:axId val="362710112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="628429872"/>
+        <c:axId val="362707760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12882,12 +12871,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="628428304"/>
+        <c:crossAx val="362710112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="628428304"/>
+        <c:axId val="362710112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12944,7 +12933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="628429872"/>
+        <c:crossAx val="362707760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13084,7 +13073,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13349,7 +13337,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>49.646959715186867</c:v>
+                  <c:v>49.585161390707462</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70.445705838563896</c:v>
@@ -13397,11 +13385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="559024632"/>
-        <c:axId val="559028160"/>
+        <c:axId val="362708544"/>
+        <c:axId val="362712856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="559024632"/>
+        <c:axId val="362708544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13458,12 +13446,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="559028160"/>
+        <c:crossAx val="362712856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="559028160"/>
+        <c:axId val="362712856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13520,7 +13508,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="559024632"/>
+        <c:crossAx val="362708544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13534,7 +13522,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13860,11 +13847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492977504"/>
-        <c:axId val="492972016"/>
+        <c:axId val="362710504"/>
+        <c:axId val="362714424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="492977504"/>
+        <c:axId val="362710504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13920,12 +13907,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492972016"/>
+        <c:crossAx val="362714424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492972016"/>
+        <c:axId val="362714424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13982,7 +13969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492977504"/>
+        <c:crossAx val="362710504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14289,11 +14276,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492975544"/>
-        <c:axId val="492975152"/>
+        <c:axId val="362711288"/>
+        <c:axId val="362709720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="492975544"/>
+        <c:axId val="362711288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14411,12 +14398,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492975152"/>
+        <c:crossAx val="362709720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492975152"/>
+        <c:axId val="362709720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14529,7 +14516,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492975544"/>
+        <c:crossAx val="362711288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -27729,8 +27716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView topLeftCell="I35" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27804,7 +27791,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>49.646959715186867</v>
+        <v>49.585161390707462</v>
       </c>
       <c r="C3" s="1">
         <v>70.445705838563896</v>
@@ -28095,8 +28082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28449,8 +28436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE73"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28710,15 +28697,14 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <f ca="1">(#REF!/B$35)*100</f>
-        <v>2.8637213569337003E-2</v>
+        <v>2.8676646875813391E-2</v>
       </c>
       <c r="C3" s="5">
         <v>0.65</v>
       </c>
       <c r="D3" s="2">
-        <f ca="1">B3*C3</f>
-        <v>1.8614188820069051E-2</v>
+        <f>B3*C3</f>
+        <v>1.8639820469278704E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -28930,15 +28916,14 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4" ca="1" si="0">(#REF!/B$35)*100</f>
-        <v>0.13942027426231718</v>
+        <v>1.4338323437906694E-3</v>
       </c>
       <c r="C4" s="5">
         <v>0.94505494505494514</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D35" ca="1" si="1">B4*C4</f>
-        <v>0.13175981963251954</v>
+        <f t="shared" ref="D4:D35" si="0">B4*C4</f>
+        <v>1.3550503468790942E-3</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -29150,15 +29135,14 @@
         <v>21</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5" ca="1" si="2">(#REF!/B$35)*100</f>
-        <v>1.8471002752222365E-2</v>
+        <v>1.8496437234899635E-2</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8471002752222365E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.8496437234899635E-2</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -29370,15 +29354,14 @@
         <v>22</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6" ca="1" si="3">(#REF!/B$35)*100</f>
-        <v>2.167264322927424E-2</v>
+        <v>2.1702486355615572E-2</v>
       </c>
       <c r="C6" s="5">
         <v>0.88636363636363635</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9209842862311258E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.9236294724295621E-2</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -29590,15 +29573,14 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7" ca="1" si="4">(#REF!/B$35)*100</f>
-        <v>7.9726002577034227E-3</v>
+        <v>7.9835784902264478E-3</v>
       </c>
       <c r="C7" s="5">
         <v>0.58333333333333337</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.6506834836603306E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.6570874526320949E-3</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -29810,15 +29792,14 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8" ca="1" si="5">(#REF!/B$35)*100</f>
-        <v>1.7840984053696953E-3</v>
+        <v>1.7865551003631742E-3</v>
       </c>
       <c r="C8" s="5">
         <v>0.9935794542536116</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7726435199419605E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.7750844416128488E-3</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -30030,15 +30011,14 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9" ca="1" si="6">(#REF!/B$35)*100</f>
-        <v>2.6761476080545427E-3</v>
+        <v>2.6798326505447609E-3</v>
       </c>
       <c r="C9" s="5">
         <v>0.9935794542536116</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.6589652799129406E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.662626662419273E-3</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -30250,15 +30230,14 @@
         <v>26</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10" ca="1" si="7">(#REF!/B$35)*100</f>
-        <v>9.5361921185892207E-4</v>
+        <v>1.4338323437906694E-3</v>
       </c>
       <c r="C10" s="5">
         <v>0.8858858858858859</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.4479780029544146E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.2702118360908333E-3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -30470,15 +30449,14 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11" ca="1" si="8">(#REF!/B$35)*100</f>
-        <v>3.0316786145178611E-2</v>
+        <v>3.0358532215079843E-2</v>
       </c>
       <c r="C11" s="5">
         <v>0.9379870589902235</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.8436753074351642E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8475910347682699E-2</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -30690,15 +30668,14 @@
         <v>28</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12" ca="1" si="9">(#REF!/B$35)*100</f>
-        <v>1.669549551092347</v>
+        <v>1.6718485128599205</v>
       </c>
       <c r="C12" s="5">
         <v>0.77778387650085756</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2985487218588723</v>
+        <f t="shared" si="0"/>
+        <v>1.3003368172543828</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -30910,15 +30887,14 @@
         <v>29</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13" ca="1" si="10">(#REF!/B$35)*100</f>
-        <v>2.7491725026563521E-4</v>
+        <v>2.7529581000780849E-4</v>
       </c>
       <c r="C13" s="5">
         <v>0.5625</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.5464095327441979E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.5485389312939226E-4</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -31130,15 +31106,14 @@
         <v>30</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14" ca="1" si="11">(#REF!/B$35)*100</f>
-        <v>6.1701368072717102</v>
+        <v>6.1786330562218144</v>
       </c>
       <c r="C14" s="5">
         <v>0.72727557531907505</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.4873897963059344</v>
+        <f t="shared" si="0"/>
+        <v>4.4935689106491754</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -31350,15 +31325,14 @@
         <v>31</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15" ca="1" si="12">(#REF!/B$35)*100</f>
-        <v>0.43960986550289227</v>
+        <v>0.44021520619061133</v>
       </c>
       <c r="C15" s="5">
         <v>0.87616441925607458</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.38517052250758266</v>
+        <f t="shared" si="0"/>
+        <v>0.38570090047969008</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -31570,15 +31544,14 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16" ca="1" si="13">(#REF!/B$35)*100</f>
-        <v>0.19587567709290818</v>
+        <v>0.19614539696587602</v>
       </c>
       <c r="C16" s="5">
         <v>0.97954648459772797</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.19186933091455791</v>
+        <f t="shared" si="0"/>
+        <v>0.19213353406794972</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -31790,15 +31763,14 @@
         <v>33</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17" ca="1" si="14">(#REF!/B$35)*100</f>
-        <v>8.3047919351077304E-2</v>
+        <v>8.3162275939858823E-2</v>
       </c>
       <c r="C17" s="5">
         <v>0.74137931034482762</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.1570009174074555E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.1654790782998785E-2</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -32010,15 +31982,14 @@
         <v>34</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18" ca="1" si="15">(#REF!/B$35)*100</f>
-        <v>2.6367800305607756</v>
+        <v>2.6404108640845805</v>
       </c>
       <c r="C18" s="5">
         <v>0.52471564035088669</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3835597222001279</v>
+        <f t="shared" si="0"/>
+        <v>1.3854648773375786</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -32230,15 +32201,14 @@
         <v>35</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19" ca="1" si="16">(#REF!/B$35)*100</f>
-        <v>1.7827137960936177</v>
+        <v>1.7851685844867287</v>
       </c>
       <c r="C19" s="5">
         <v>0.73452671535613911</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3094509090647188</v>
+        <f t="shared" si="0"/>
+        <v>1.3112540167200051</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -32450,15 +32420,14 @@
         <v>36</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20" ca="1" si="17">(#REF!/B$35)*100</f>
-        <v>1.4603275006154495</v>
+        <v>1.4623383646175718</v>
       </c>
       <c r="C20" s="5">
         <v>0.4912337811960415</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.71736219991189187</v>
+        <f t="shared" si="0"/>
+        <v>0.71835000423912543</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -32670,15 +32639,14 @@
         <v>37</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21" ca="1" si="18">(#REF!/B$35)*100</f>
-        <v>4.5699107909273353</v>
+        <v>4.5762035362865188</v>
       </c>
       <c r="C21" s="5">
         <v>0.76631483565083092</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.5019904366884398</v>
+        <f t="shared" si="0"/>
+        <v>3.506812660814155</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -32890,15 +32858,14 @@
         <v>38</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22" ca="1" si="19">(#REF!/B$35)*100</f>
-        <v>0.127335370136057</v>
+        <v>0.12751071033330424</v>
       </c>
       <c r="C22" s="5">
         <v>0.96705273810862469</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.12314001834814912</v>
+        <f t="shared" si="0"/>
+        <v>0.12330958156599757</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -33110,15 +33077,14 @@
         <v>39</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23" ca="1" si="20">(#REF!/B$35)*100</f>
-        <v>0.96029168262057774</v>
+        <v>0.9616139996866504</v>
       </c>
       <c r="C23" s="5">
         <v>0.70029523156293794</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.67248768624874078</v>
+        <f t="shared" si="0"/>
+        <v>0.67341369858472577</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -33330,15 +33296,14 @@
         <v>40</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24" ca="1" si="21">(#REF!/B$35)*100</f>
-        <v>1.8090657600201214</v>
+        <v>1.811556834941852</v>
       </c>
       <c r="C24" s="5">
         <v>0.68664682132943711</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2421892536937387</v>
+        <f t="shared" si="0"/>
+        <v>1.2438997423704385</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -33550,15 +33515,14 @@
         <v>41</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25" ca="1" si="22">(#REF!/B$35)*100</f>
-        <v>7.7005467287947198E-3</v>
+        <v>7.7111503449062216E-3</v>
       </c>
       <c r="C25" s="5">
         <v>0.51803644477500932</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.9891638502086444E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.9946569098008059E-3</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -33770,15 +33734,14 @@
         <v>42</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26" ca="1" si="23">(#REF!/B$35)*100</f>
-        <v>31.258532368291696</v>
+        <v>31.301575218249724</v>
       </c>
       <c r="C26" s="5">
         <v>0.52182050165299265</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>16.311343041358281</v>
+        <f t="shared" si="0"/>
+        <v>16.333803682915953</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -33990,15 +33953,14 @@
         <v>43</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27" ca="1" si="24">(#REF!/B$35)*100</f>
-        <v>0.51268630708912644</v>
+        <v>0.51339227368831197</v>
       </c>
       <c r="C27" s="5">
         <v>0.67819558951672365</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.34770159227346215</v>
+        <f t="shared" si="0"/>
+        <v>0.34818037570737587</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -34210,15 +34172,14 @@
         <v>44</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28" ca="1" si="25">(#REF!/B$35)*100</f>
-        <v>3.6101732383893239</v>
+        <v>3.6151444297169153</v>
       </c>
       <c r="C28" s="5">
         <v>0.57076383920143292</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.0605563377253606</v>
+        <f t="shared" si="0"/>
+        <v>2.0633937139729013</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -34430,15 +34391,14 @@
         <v>45</v>
       </c>
       <c r="B29">
-        <f t="shared" ref="B29" ca="1" si="26">(#REF!/B$35)*100</f>
-        <v>3.2140547091341833</v>
+        <v>3.2184804471366011</v>
       </c>
       <c r="C29" s="5">
         <v>0.4119287022145795</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.323961385180302</v>
+        <f t="shared" si="0"/>
+        <v>1.3257844736919797</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -34650,15 +34610,14 @@
         <v>46</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30" ca="1" si="27">(#REF!/B$35)*100</f>
-        <v>2.0184811116886121</v>
+        <v>2.0212605505506125</v>
       </c>
       <c r="C30" s="5">
         <v>0.60908383468433869</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2294242157452069</v>
+        <f t="shared" si="0"/>
+        <v>1.2311171270255448</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -34861,15 +34820,14 @@
         <v>47</v>
       </c>
       <c r="B31">
-        <f t="shared" ref="B31" ca="1" si="28">(#REF!/B$35)*100</f>
-        <v>5.0179457246623276</v>
+        <v>5.0248554119879953</v>
       </c>
       <c r="C31" s="5">
         <v>0.4164950536354331</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.0899495737329286</v>
+        <f t="shared" si="0"/>
+        <v>2.0928274243262366</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -35063,15 +35021,14 @@
         <v>48</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32" ca="1" si="29">(#REF!/B$35)*100</f>
-        <v>0.6434667340175747</v>
+        <v>0.6443527846407765</v>
       </c>
       <c r="C32" s="5">
         <v>0.85671307010360664</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.55126636120973727</v>
+        <f t="shared" si="0"/>
+        <v>0.5520254523594077</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -35265,15 +35222,14 @@
         <v>49</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33" ca="1" si="30">(#REF!/B$35)*100</f>
-        <v>21.855786801214222</v>
+        <v>21.885882115380461</v>
       </c>
       <c r="C33" s="5">
         <v>0.24939507620133408</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.4507256147289329</v>
+        <f t="shared" si="0"/>
+        <v>5.4582312378987252</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -35452,15 +35408,14 @@
         <v>50</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34" ca="1" si="31">(#REF!/B$35)*100</f>
-        <v>5.6719480895520622</v>
+        <v>5.6797583350143839</v>
       </c>
       <c r="C34" s="5">
         <v>0.60192974780895803</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.4141142831295741</v>
+        <f t="shared" si="0"/>
+        <v>3.4188155022110354</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -35600,15 +35555,14 @@
         <v>51</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35" ca="1" si="32">(#REF!/B$35)*100</f>
-        <v>4.0324003152556296</v>
+        <v>4.0379529112539085</v>
       </c>
       <c r="C35" s="5">
         <v>0.31312025157339896</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.262626201157496</v>
+        <f t="shared" si="0"/>
+        <v>1.2643648314133626</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -35718,8 +35672,8 @@
     </row>
     <row r="36" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
-        <f ca="1">SUM(D3:D35)</f>
-        <v>49.646959715186867</v>
+        <f>SUM(D3:D35)</f>
+        <v>49.585161390707462</v>
       </c>
       <c r="E36">
         <v>40</v>
@@ -36146,6 +36100,9 @@
       </c>
     </row>
     <row r="43" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>1003</v>
+      </c>
       <c r="BA43">
         <v>98.281575126903107</v>
       </c>
@@ -36760,11 +36717,11 @@
         <v>49.148754824102483</v>
       </c>
       <c r="CD73" s="1">
-        <f t="shared" ref="CD73:CE73" si="33">SUM(CD3:CD72)</f>
+        <f t="shared" ref="CD73:CE73" si="1">SUM(CD3:CD72)</f>
         <v>167</v>
       </c>
       <c r="CE73" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="1"/>
         <v>157</v>
       </c>
     </row>

</xml_diff>